<commit_message>
reloading car brands after change data from a paint
</commit_message>
<xml_diff>
--- a/assets/files/Inventary_bu.xlsx
+++ b/assets/files/Inventary_bu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L03540110\Documents\dev\paintCodes\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DF7574-AF52-4DA7-847E-70C7666D5C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAF858F-13B5-41DD-971B-B7BC6ED9850E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3586,7 +3586,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0_ "/>
-    <numFmt numFmtId="166" formatCode="#,##0.000_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.000_ "/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -3687,7 +3687,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5752,7 +5752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="2" customFormat="1" ht="43.2">
+    <row r="34" spans="1:16" s="2" customFormat="1" ht="72">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="2" customFormat="1" ht="43.2">
+    <row r="36" spans="1:16" s="2" customFormat="1" ht="57.6">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="2" customFormat="1" ht="28.8">
+    <row r="64" spans="1:16" s="2" customFormat="1" ht="43.2">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="2" customFormat="1" ht="57.6">
+    <row r="73" spans="1:16" s="2" customFormat="1" ht="86.4">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="2" customFormat="1">
+    <row r="85" spans="1:16" s="2" customFormat="1" ht="28.8">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:16" s="2" customFormat="1" ht="28.8">
+    <row r="102" spans="1:16" s="2" customFormat="1" ht="43.2">
       <c r="A102" s="2">
         <v>100</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" ht="28.8">
       <c r="A177" s="2">
         <v>175</v>
       </c>
@@ -14719,7 +14719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:16">
+    <row r="210" spans="1:16" ht="28.8">
       <c r="A210" s="2">
         <v>208</v>
       </c>
@@ -15229,7 +15229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" ht="28.8">
       <c r="A220" s="2">
         <v>218</v>
       </c>
@@ -15382,7 +15382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" ht="28.8">
       <c r="A223" s="2">
         <v>221</v>
       </c>
@@ -26331,6 +26331,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="K1:K2"/>
@@ -26339,12 +26345,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>